<commit_message>
testing #1 - fail
</commit_message>
<xml_diff>
--- a/assets/qt_schedule.xlsx
+++ b/assets/qt_schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mayer\android_apps\daily_qt_hl\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2F05AB-46FD-444D-871F-209AC77EC983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E620C92-5485-4DFB-B8EE-FAC407F111C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-106" yWindow="-106" windowWidth="22875" windowHeight="12358" xr2:uid="{03EA6E69-C154-4164-AD29-32C70FF0EC51}"/>
   </bookViews>
@@ -2023,13 +2023,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{565C5AE5-7EBE-4A4A-BD63-5A68899D1B94}">
   <dimension ref="A1:E368"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="D139" sqref="D139"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.19921875" customWidth="1"/>
     <col min="2" max="2" width="13.09765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.19921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.3984375" bestFit="1" customWidth="1"/>

</xml_diff>